<commit_message>
[EDP-DDM-28147] Registry services requirements.
Change-Id: Ib1a33727e573f0bcbda223acc60eb60aba9e7292
</commit_message>
<xml_diff>
--- a/docs/ua/modules/arch/attachments/architecture/platform-system-requirements/registry-resources.xlsx
+++ b/docs/ua/modules/arch/attachments/architecture/platform-system-requirements/registry-resources.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Maksym_Kharchenko/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Maksym_Kharchenko/Work/Development/mdtu-ddm/mdtu-ddm-gerrit-workspace/mdtu-ddm/general/ddm-architecture/docs/ua/modules/arch/attachments/architecture/platform-system-requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A9C770-4D25-9741-B108-599B8657515C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D966C3E-2F98-AA4E-8DB0-3BC59D58316C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{76BACE1B-BDCC-F34F-9205-7BB42BE8027F}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="47160" windowHeight="21580" xr2:uid="{76BACE1B-BDCC-F34F-9205-7BB42BE8027F}"/>
   </bookViews>
   <sheets>
     <sheet name="Registry Resources" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="110">
   <si>
     <t>Technology</t>
   </si>
@@ -314,39 +314,9 @@
     <t>Підсистема управління нереляційними базами даних</t>
   </si>
   <si>
-    <t>Service Mesh member</t>
-  </si>
-  <si>
     <t>Java</t>
   </si>
   <si>
-    <t>-Xms</t>
-  </si>
-  <si>
-    <t>-Xmx</t>
-  </si>
-  <si>
-    <t>1536m</t>
-  </si>
-  <si>
-    <t>768m</t>
-  </si>
-  <si>
-    <t>512m</t>
-  </si>
-  <si>
-    <t>1200m</t>
-  </si>
-  <si>
-    <t>128m</t>
-  </si>
-  <si>
-    <t>330m</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -359,13 +329,43 @@
     <t>Zone</t>
   </si>
   <si>
-    <t>Criticality</t>
-  </si>
-  <si>
-    <t>non-critical</t>
-  </si>
-  <si>
-    <t>critical</t>
+    <t>Service Mesh</t>
+  </si>
+  <si>
+    <t>Monitoring</t>
+  </si>
+  <si>
+    <t>Java Opts</t>
+  </si>
+  <si>
+    <t>-XX:+ExplicitGCInvokesConcurrent -XX:+AlwaysPreTouch -XX:+UseG1GC</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -XX:+AlwaysPreTouch -XX:+UseG1GC</t>
+  </si>
+  <si>
+    <t>-Duser.timezone=UTC</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -Duser.timezone=UTC</t>
+  </si>
+  <si>
+    <t>-XX:+AlwaysPreTouch -XX:+UseG1GC</t>
+  </si>
+  <si>
+    <t>-Xms, Mb</t>
+  </si>
+  <si>
+    <t>-Xmx, Mb</t>
+  </si>
+  <si>
+    <t>-Xmn, Mb</t>
+  </si>
+  <si>
+    <t>Deployment Mode</t>
+  </si>
+  <si>
+    <t>Min Profile</t>
   </si>
 </sst>
 </file>
@@ -443,7 +443,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -452,11 +452,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -470,18 +483,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{06C99DE8-B980-0548-85E0-AAF92621FDD9}" name="Table3" displayName="Table3" ref="A1:I65" totalsRowShown="0">
-  <autoFilter ref="A1:I65" xr:uid="{06C99DE8-B980-0548-85E0-AAF92621FDD9}"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{06C99DE8-B980-0548-85E0-AAF92621FDD9}" name="Table3" displayName="Table3" ref="A1:M65" totalsRowShown="0">
+  <autoFilter ref="A1:M65" xr:uid="{06C99DE8-B980-0548-85E0-AAF92621FDD9}"/>
+  <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{7B40E2F0-02D6-904B-8018-66FABFA0DD1D}" name="Zone"/>
     <tableColumn id="2" xr3:uid="{9B6E3613-3147-0A49-A88D-DE5E5756377A}" name="Subsystem"/>
     <tableColumn id="3" xr3:uid="{7B693F86-BB20-4643-8C59-CE9AAFCBF004}" name="Component"/>
     <tableColumn id="4" xr3:uid="{BDC056D6-A828-3747-8D2F-B230006DB630}" name="Type"/>
-    <tableColumn id="9" xr3:uid="{26E395E2-1F19-C84B-980C-08C4B5582553}" name="Criticality"/>
-    <tableColumn id="5" xr3:uid="{E36D12C6-BEC1-3841-BB7F-07B8DD85B728}" name="Service Mesh member"/>
+    <tableColumn id="9" xr3:uid="{26E395E2-1F19-C84B-980C-08C4B5582553}" name="Deployment Mode"/>
+    <tableColumn id="14" xr3:uid="{206BB385-4C22-624D-A2DB-36D434439669}" name="Min Profile" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{E36D12C6-BEC1-3841-BB7F-07B8DD85B728}" name="Service Mesh" dataDxfId="0"/>
+    <tableColumn id="11" xr3:uid="{DE3293B1-99DC-3448-B36C-7DC56C231CB7}" name="Monitoring"/>
     <tableColumn id="6" xr3:uid="{90E59384-34DA-9D4D-8715-BED9DC803BBE}" name="Technology"/>
-    <tableColumn id="7" xr3:uid="{7D3E02CE-7CDD-5E44-88DF-1162888AE695}" name="-Xms"/>
-    <tableColumn id="8" xr3:uid="{3D28B649-AB9D-9C49-8889-6B0D4888A8D3}" name="-Xmx"/>
+    <tableColumn id="7" xr3:uid="{7D3E02CE-7CDD-5E44-88DF-1162888AE695}" name="-Xms, Mb"/>
+    <tableColumn id="8" xr3:uid="{3D28B649-AB9D-9C49-8889-6B0D4888A8D3}" name="-Xmx, Mb"/>
+    <tableColumn id="13" xr3:uid="{729BA2AA-0236-6D4E-88FA-AF5279155852}" name="-Xmn, Mb"/>
+    <tableColumn id="12" xr3:uid="{84FF7781-94A1-1246-98C1-52FEAF154639}" name="Java Opts"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -784,10 +801,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C809D083-7CF6-1445-A306-E810BD791428}">
-  <dimension ref="A1:I65"/>
+  <dimension ref="A1:M65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -796,42 +813,57 @@
     <col min="2" max="2" width="65.83203125" customWidth="1"/>
     <col min="3" max="3" width="35.5" customWidth="1"/>
     <col min="4" max="5" width="19.6640625" customWidth="1"/>
-    <col min="6" max="6" width="25" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" customWidth="1"/>
-    <col min="8" max="8" width="13.5" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="15.5" style="6" customWidth="1"/>
+    <col min="8" max="8" width="15.5" customWidth="1"/>
     <col min="9" max="9" width="14.33203125" customWidth="1"/>
+    <col min="10" max="10" width="13.5" customWidth="1"/>
+    <col min="11" max="12" width="14.33203125" customWidth="1"/>
+    <col min="13" max="13" width="60.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="L1" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="F1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -844,14 +876,14 @@
       <c r="D2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
-        <v>108</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>73</v>
       </c>
@@ -864,14 +896,14 @@
       <c r="D3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
-        <v>108</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -884,14 +916,14 @@
       <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
-        <v>108</v>
-      </c>
-      <c r="F4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>73</v>
       </c>
@@ -904,14 +936,14 @@
       <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="E5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>73</v>
       </c>
@@ -924,23 +956,29 @@
       <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="E6" t="s">
-        <v>108</v>
-      </c>
-      <c r="F6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" t="s">
-        <v>93</v>
-      </c>
-      <c r="H6" t="s">
-        <v>102</v>
-      </c>
-      <c r="I6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>73</v>
       </c>
@@ -953,14 +991,14 @@
       <c r="D7" t="s">
         <v>15</v>
       </c>
-      <c r="E7" t="s">
-        <v>108</v>
-      </c>
-      <c r="F7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>73</v>
       </c>
@@ -973,14 +1011,14 @@
       <c r="D8" t="s">
         <v>15</v>
       </c>
-      <c r="E8" t="s">
-        <v>108</v>
-      </c>
-      <c r="F8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F8" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>73</v>
       </c>
@@ -993,14 +1031,14 @@
       <c r="D9" t="s">
         <v>15</v>
       </c>
-      <c r="E9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>73</v>
       </c>
@@ -1013,14 +1051,14 @@
       <c r="D10" t="s">
         <v>15</v>
       </c>
-      <c r="E10" t="s">
-        <v>108</v>
-      </c>
-      <c r="F10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F10" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>73</v>
       </c>
@@ -1033,23 +1071,29 @@
       <c r="D11" t="s">
         <v>15</v>
       </c>
-      <c r="E11" t="s">
-        <v>108</v>
-      </c>
-      <c r="F11" t="s">
-        <v>3</v>
-      </c>
-      <c r="G11" t="s">
-        <v>93</v>
-      </c>
-      <c r="H11" t="s">
-        <v>102</v>
-      </c>
-      <c r="I11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F11" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>73</v>
       </c>
@@ -1062,14 +1106,29 @@
       <c r="D12" t="s">
         <v>15</v>
       </c>
-      <c r="E12" t="s">
-        <v>108</v>
-      </c>
-      <c r="F12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F12" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>73</v>
       </c>
@@ -1082,14 +1141,14 @@
       <c r="D13" t="s">
         <v>15</v>
       </c>
-      <c r="E13" t="s">
-        <v>108</v>
-      </c>
-      <c r="F13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F13" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>73</v>
       </c>
@@ -1102,14 +1161,14 @@
       <c r="D14" t="s">
         <v>15</v>
       </c>
-      <c r="E14" t="s">
-        <v>108</v>
-      </c>
-      <c r="F14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F14" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>73</v>
       </c>
@@ -1122,23 +1181,29 @@
       <c r="D15" t="s">
         <v>15</v>
       </c>
-      <c r="E15" t="s">
-        <v>108</v>
-      </c>
-      <c r="F15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G15" t="s">
-        <v>93</v>
-      </c>
-      <c r="H15" t="s">
-        <v>98</v>
-      </c>
-      <c r="I15" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F15" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J15" s="6">
+        <v>512</v>
+      </c>
+      <c r="K15" s="6">
+        <v>512</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>73</v>
       </c>
@@ -1151,14 +1216,29 @@
       <c r="D16" t="s">
         <v>15</v>
       </c>
-      <c r="E16" t="s">
-        <v>108</v>
-      </c>
-      <c r="F16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F16" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>73</v>
       </c>
@@ -1171,14 +1251,14 @@
       <c r="D17" t="s">
         <v>15</v>
       </c>
-      <c r="E17" t="s">
-        <v>108</v>
-      </c>
-      <c r="F17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F17" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>74</v>
       </c>
@@ -1191,14 +1271,14 @@
       <c r="D18" t="s">
         <v>15</v>
       </c>
-      <c r="E18" t="s">
-        <v>109</v>
-      </c>
-      <c r="F18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F18" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>74</v>
       </c>
@@ -1211,14 +1291,14 @@
       <c r="D19" t="s">
         <v>15</v>
       </c>
-      <c r="E19" t="s">
-        <v>109</v>
-      </c>
-      <c r="F19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F19" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>74</v>
       </c>
@@ -1231,14 +1311,14 @@
       <c r="D20" t="s">
         <v>15</v>
       </c>
-      <c r="E20" t="s">
-        <v>109</v>
-      </c>
-      <c r="F20" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F20" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>74</v>
       </c>
@@ -1251,14 +1331,14 @@
       <c r="D21" t="s">
         <v>15</v>
       </c>
-      <c r="E21" t="s">
-        <v>109</v>
-      </c>
-      <c r="F21" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F21" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>74</v>
       </c>
@@ -1271,23 +1351,29 @@
       <c r="D22" t="s">
         <v>15</v>
       </c>
-      <c r="E22" t="s">
-        <v>109</v>
-      </c>
-      <c r="F22" t="s">
-        <v>3</v>
-      </c>
-      <c r="G22" t="s">
-        <v>93</v>
-      </c>
-      <c r="H22" t="s">
-        <v>96</v>
-      </c>
-      <c r="I22" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F22" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J22" s="6">
+        <v>1536</v>
+      </c>
+      <c r="K22" s="6">
+        <v>1536</v>
+      </c>
+      <c r="L22" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M22" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>74</v>
       </c>
@@ -1300,20 +1386,29 @@
       <c r="D23" t="s">
         <v>15</v>
       </c>
-      <c r="F23" t="s">
-        <v>3</v>
-      </c>
-      <c r="G23" t="s">
-        <v>93</v>
-      </c>
-      <c r="H23" t="s">
-        <v>98</v>
-      </c>
-      <c r="I23" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F23" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J23" s="6">
+        <v>512</v>
+      </c>
+      <c r="K23" s="6">
+        <v>512</v>
+      </c>
+      <c r="L23" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>74</v>
       </c>
@@ -1326,23 +1421,29 @@
       <c r="D24" t="s">
         <v>15</v>
       </c>
-      <c r="E24" t="s">
-        <v>109</v>
-      </c>
-      <c r="F24" t="s">
-        <v>3</v>
-      </c>
-      <c r="G24" t="s">
-        <v>93</v>
-      </c>
-      <c r="H24" t="s">
-        <v>102</v>
-      </c>
-      <c r="I24" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F24" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L24" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>74</v>
       </c>
@@ -1355,14 +1456,14 @@
       <c r="D25" t="s">
         <v>15</v>
       </c>
-      <c r="E25" t="s">
-        <v>109</v>
-      </c>
-      <c r="F25" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F25" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>74</v>
       </c>
@@ -1375,23 +1476,29 @@
       <c r="D26" t="s">
         <v>15</v>
       </c>
-      <c r="E26" t="s">
-        <v>109</v>
-      </c>
-      <c r="F26" t="s">
-        <v>3</v>
-      </c>
-      <c r="G26" t="s">
-        <v>93</v>
-      </c>
-      <c r="H26" t="s">
-        <v>101</v>
-      </c>
-      <c r="I26" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F26" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J26" s="6">
+        <v>330</v>
+      </c>
+      <c r="K26" s="6">
+        <v>330</v>
+      </c>
+      <c r="L26" s="6">
+        <v>200</v>
+      </c>
+      <c r="M26" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>74</v>
       </c>
@@ -1404,23 +1511,29 @@
       <c r="D27" t="s">
         <v>15</v>
       </c>
-      <c r="E27" t="s">
-        <v>109</v>
-      </c>
-      <c r="F27" t="s">
-        <v>3</v>
-      </c>
-      <c r="G27" t="s">
-        <v>93</v>
-      </c>
-      <c r="H27" t="s">
-        <v>101</v>
-      </c>
-      <c r="I27" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F27" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J27" s="6">
+        <v>330</v>
+      </c>
+      <c r="K27" s="6">
+        <v>330</v>
+      </c>
+      <c r="L27" s="6">
+        <v>200</v>
+      </c>
+      <c r="M27" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>74</v>
       </c>
@@ -1433,23 +1546,29 @@
       <c r="D28" t="s">
         <v>15</v>
       </c>
-      <c r="E28" t="s">
-        <v>109</v>
-      </c>
-      <c r="F28" t="s">
-        <v>3</v>
-      </c>
-      <c r="G28" t="s">
-        <v>93</v>
-      </c>
-      <c r="H28" t="s">
-        <v>98</v>
-      </c>
-      <c r="I28" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F28" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J28" s="6">
+        <v>512</v>
+      </c>
+      <c r="K28" s="6">
+        <v>512</v>
+      </c>
+      <c r="L28" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>74</v>
       </c>
@@ -1462,23 +1581,29 @@
       <c r="D29" t="s">
         <v>15</v>
       </c>
-      <c r="E29" t="s">
-        <v>109</v>
-      </c>
-      <c r="F29" t="s">
-        <v>3</v>
-      </c>
-      <c r="G29" t="s">
-        <v>93</v>
-      </c>
-      <c r="H29" t="s">
-        <v>98</v>
-      </c>
-      <c r="I29" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F29" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J29" s="6">
+        <v>512</v>
+      </c>
+      <c r="K29" s="6">
+        <v>512</v>
+      </c>
+      <c r="L29" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>74</v>
       </c>
@@ -1491,23 +1616,29 @@
       <c r="D30" t="s">
         <v>15</v>
       </c>
-      <c r="E30" t="s">
-        <v>109</v>
-      </c>
-      <c r="F30" t="s">
-        <v>3</v>
-      </c>
-      <c r="G30" t="s">
-        <v>93</v>
-      </c>
-      <c r="H30" t="s">
-        <v>99</v>
-      </c>
-      <c r="I30" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F30" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J30" s="6">
+        <v>1200</v>
+      </c>
+      <c r="K30" s="6">
+        <v>1200</v>
+      </c>
+      <c r="L30" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M30" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>74</v>
       </c>
@@ -1520,23 +1651,29 @@
       <c r="D31" t="s">
         <v>15</v>
       </c>
-      <c r="E31" t="s">
-        <v>109</v>
-      </c>
-      <c r="F31" t="s">
-        <v>3</v>
-      </c>
-      <c r="G31" t="s">
-        <v>93</v>
-      </c>
-      <c r="H31" t="s">
-        <v>99</v>
-      </c>
-      <c r="I31" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F31" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J31" s="6">
+        <v>1200</v>
+      </c>
+      <c r="K31" s="6">
+        <v>1200</v>
+      </c>
+      <c r="L31" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M31" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>74</v>
       </c>
@@ -1549,14 +1686,14 @@
       <c r="D32" t="s">
         <v>15</v>
       </c>
-      <c r="E32" t="s">
-        <v>109</v>
-      </c>
-      <c r="F32" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F32" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>74</v>
       </c>
@@ -1569,14 +1706,14 @@
       <c r="D33" t="s">
         <v>2</v>
       </c>
-      <c r="E33" t="s">
-        <v>109</v>
-      </c>
-      <c r="F33" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F33" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>74</v>
       </c>
@@ -1589,14 +1726,14 @@
       <c r="D34" t="s">
         <v>2</v>
       </c>
-      <c r="E34" t="s">
-        <v>109</v>
-      </c>
-      <c r="F34" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F34" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>74</v>
       </c>
@@ -1609,14 +1746,14 @@
       <c r="D35" t="s">
         <v>15</v>
       </c>
-      <c r="E35" t="s">
-        <v>109</v>
-      </c>
-      <c r="F35" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F35" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>74</v>
       </c>
@@ -1629,14 +1766,14 @@
       <c r="D36" t="s">
         <v>15</v>
       </c>
-      <c r="E36" t="s">
-        <v>109</v>
-      </c>
-      <c r="F36" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F36" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>74</v>
       </c>
@@ -1649,14 +1786,14 @@
       <c r="D37" t="s">
         <v>15</v>
       </c>
-      <c r="E37" t="s">
-        <v>109</v>
-      </c>
-      <c r="F37" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F37" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>74</v>
       </c>
@@ -1669,23 +1806,29 @@
       <c r="D38" t="s">
         <v>15</v>
       </c>
-      <c r="E38" t="s">
-        <v>109</v>
-      </c>
-      <c r="F38" t="s">
-        <v>3</v>
-      </c>
-      <c r="G38" t="s">
-        <v>93</v>
-      </c>
-      <c r="H38" t="s">
-        <v>98</v>
-      </c>
-      <c r="I38" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F38" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I38" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J38" s="6">
+        <v>512</v>
+      </c>
+      <c r="K38" s="6">
+        <v>512</v>
+      </c>
+      <c r="L38" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>74</v>
       </c>
@@ -1698,23 +1841,29 @@
       <c r="D39" t="s">
         <v>15</v>
       </c>
-      <c r="E39" t="s">
-        <v>109</v>
-      </c>
-      <c r="F39" t="s">
-        <v>3</v>
-      </c>
-      <c r="G39" t="s">
-        <v>93</v>
-      </c>
-      <c r="H39" t="s">
-        <v>101</v>
-      </c>
-      <c r="I39" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F39" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I39" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J39" s="6">
+        <v>330</v>
+      </c>
+      <c r="K39" s="6">
+        <v>330</v>
+      </c>
+      <c r="L39" s="6">
+        <v>200</v>
+      </c>
+      <c r="M39" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>74</v>
       </c>
@@ -1727,23 +1876,29 @@
       <c r="D40" t="s">
         <v>15</v>
       </c>
-      <c r="E40" t="s">
-        <v>109</v>
-      </c>
-      <c r="F40" t="s">
-        <v>3</v>
-      </c>
-      <c r="G40" t="s">
-        <v>93</v>
-      </c>
-      <c r="H40" t="s">
-        <v>99</v>
-      </c>
-      <c r="I40" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F40" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I40" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J40" s="6">
+        <v>1200</v>
+      </c>
+      <c r="K40" s="6">
+        <v>1200</v>
+      </c>
+      <c r="L40" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M40" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>74</v>
       </c>
@@ -1756,23 +1911,29 @@
       <c r="D41" t="s">
         <v>15</v>
       </c>
-      <c r="E41" t="s">
-        <v>109</v>
-      </c>
-      <c r="F41" t="s">
-        <v>3</v>
-      </c>
-      <c r="G41" t="s">
-        <v>93</v>
-      </c>
-      <c r="H41" t="s">
-        <v>99</v>
-      </c>
-      <c r="I41" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F41" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I41" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J41" s="6">
+        <v>1200</v>
+      </c>
+      <c r="K41" s="6">
+        <v>1200</v>
+      </c>
+      <c r="L41" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M41" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>74</v>
       </c>
@@ -1785,23 +1946,29 @@
       <c r="D42" t="s">
         <v>15</v>
       </c>
-      <c r="E42" t="s">
-        <v>109</v>
-      </c>
-      <c r="F42" t="s">
-        <v>3</v>
-      </c>
-      <c r="G42" t="s">
-        <v>93</v>
-      </c>
-      <c r="H42" t="s">
+      <c r="F42" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I42" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J42" s="6">
+        <v>128</v>
+      </c>
+      <c r="K42" s="6">
+        <v>128</v>
+      </c>
+      <c r="L42" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M42" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="I42" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>74</v>
       </c>
@@ -1814,14 +1981,29 @@
       <c r="D43" t="s">
         <v>15</v>
       </c>
-      <c r="E43" t="s">
-        <v>108</v>
-      </c>
-      <c r="F43" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F43" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I43" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J43" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K43" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L43" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M43" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>74</v>
       </c>
@@ -1834,23 +2016,29 @@
       <c r="D44" t="s">
         <v>15</v>
       </c>
-      <c r="E44" t="s">
-        <v>109</v>
-      </c>
-      <c r="F44" t="s">
-        <v>3</v>
-      </c>
-      <c r="G44" t="s">
-        <v>93</v>
-      </c>
-      <c r="H44" t="s">
-        <v>101</v>
-      </c>
-      <c r="I44" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F44" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I44" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J44" s="6">
+        <v>330</v>
+      </c>
+      <c r="K44" s="6">
+        <v>330</v>
+      </c>
+      <c r="L44" s="6">
+        <v>200</v>
+      </c>
+      <c r="M44" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>74</v>
       </c>
@@ -1863,23 +2051,29 @@
       <c r="D45" t="s">
         <v>15</v>
       </c>
-      <c r="E45" t="s">
-        <v>109</v>
-      </c>
-      <c r="F45" t="s">
-        <v>3</v>
-      </c>
-      <c r="G45" t="s">
-        <v>93</v>
-      </c>
-      <c r="H45" t="s">
+      <c r="F45" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I45" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J45" s="6">
+        <v>330</v>
+      </c>
+      <c r="K45" s="6">
+        <v>330</v>
+      </c>
+      <c r="L45" s="6">
+        <v>200</v>
+      </c>
+      <c r="M45" t="s">
         <v>101</v>
       </c>
-      <c r="I45" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>74</v>
       </c>
@@ -1892,23 +2086,29 @@
       <c r="D46" t="s">
         <v>15</v>
       </c>
-      <c r="E46" t="s">
-        <v>109</v>
-      </c>
-      <c r="F46" t="s">
-        <v>3</v>
-      </c>
-      <c r="G46" t="s">
-        <v>93</v>
-      </c>
-      <c r="H46" t="s">
+      <c r="F46" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I46" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J46" s="6">
+        <v>330</v>
+      </c>
+      <c r="K46" s="6">
+        <v>330</v>
+      </c>
+      <c r="L46" s="6">
+        <v>200</v>
+      </c>
+      <c r="M46" t="s">
         <v>101</v>
       </c>
-      <c r="I46" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>74</v>
       </c>
@@ -1921,23 +2121,29 @@
       <c r="D47" t="s">
         <v>15</v>
       </c>
-      <c r="E47" t="s">
-        <v>109</v>
-      </c>
-      <c r="F47" t="s">
-        <v>3</v>
-      </c>
-      <c r="G47" t="s">
-        <v>93</v>
-      </c>
-      <c r="H47" t="s">
+      <c r="F47" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I47" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J47" s="6">
+        <v>330</v>
+      </c>
+      <c r="K47" s="6">
+        <v>330</v>
+      </c>
+      <c r="L47" s="6">
+        <v>200</v>
+      </c>
+      <c r="M47" t="s">
         <v>101</v>
       </c>
-      <c r="I47" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>74</v>
       </c>
@@ -1950,23 +2156,29 @@
       <c r="D48" t="s">
         <v>15</v>
       </c>
-      <c r="E48" t="s">
-        <v>109</v>
-      </c>
-      <c r="F48" t="s">
-        <v>3</v>
-      </c>
-      <c r="G48" t="s">
-        <v>93</v>
-      </c>
-      <c r="H48" t="s">
-        <v>102</v>
-      </c>
-      <c r="I48" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F48" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G48" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I48" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J48" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K48" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L48" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M48" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>74</v>
       </c>
@@ -1979,14 +2191,29 @@
       <c r="D49" t="s">
         <v>15</v>
       </c>
-      <c r="E49" t="s">
-        <v>109</v>
-      </c>
-      <c r="F49" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F49" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G49" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I49" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J49" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K49" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L49" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M49" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>74</v>
       </c>
@@ -1999,14 +2226,14 @@
       <c r="D50" t="s">
         <v>15</v>
       </c>
-      <c r="E50" t="s">
-        <v>109</v>
-      </c>
-      <c r="F50" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F50" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>74</v>
       </c>
@@ -2019,14 +2246,14 @@
       <c r="D51" t="s">
         <v>15</v>
       </c>
-      <c r="E51" t="s">
-        <v>109</v>
-      </c>
-      <c r="F51" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F51" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>74</v>
       </c>
@@ -2039,23 +2266,29 @@
       <c r="D52" t="s">
         <v>15</v>
       </c>
-      <c r="E52" t="s">
-        <v>109</v>
-      </c>
-      <c r="F52" t="s">
-        <v>3</v>
-      </c>
-      <c r="G52" t="s">
-        <v>93</v>
-      </c>
-      <c r="H52" t="s">
+      <c r="F52" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I52" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J52" s="6">
+        <v>330</v>
+      </c>
+      <c r="K52" s="6">
+        <v>330</v>
+      </c>
+      <c r="L52" s="6">
+        <v>200</v>
+      </c>
+      <c r="M52" t="s">
         <v>101</v>
       </c>
-      <c r="I52" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>74</v>
       </c>
@@ -2068,23 +2301,29 @@
       <c r="D53" t="s">
         <v>15</v>
       </c>
-      <c r="E53" t="s">
-        <v>109</v>
-      </c>
-      <c r="F53" t="s">
-        <v>9</v>
-      </c>
-      <c r="G53" t="s">
-        <v>93</v>
-      </c>
-      <c r="H53" t="s">
-        <v>97</v>
+      <c r="F53" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G53" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="I53" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+      <c r="J53" s="6">
+        <v>768</v>
+      </c>
+      <c r="K53" s="6">
+        <v>768</v>
+      </c>
+      <c r="L53" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M53" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>74</v>
       </c>
@@ -2097,14 +2336,14 @@
       <c r="D54" t="s">
         <v>2</v>
       </c>
-      <c r="E54" t="s">
-        <v>109</v>
-      </c>
-      <c r="F54" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F54" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G54" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>74</v>
       </c>
@@ -2117,14 +2356,14 @@
       <c r="D55" t="s">
         <v>15</v>
       </c>
-      <c r="E55" t="s">
-        <v>109</v>
-      </c>
-      <c r="F55" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F55" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>74</v>
       </c>
@@ -2137,14 +2376,14 @@
       <c r="D56" t="s">
         <v>15</v>
       </c>
-      <c r="E56" t="s">
-        <v>109</v>
-      </c>
-      <c r="F56" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F56" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>74</v>
       </c>
@@ -2157,14 +2396,14 @@
       <c r="D57" t="s">
         <v>2</v>
       </c>
-      <c r="E57" t="s">
-        <v>109</v>
-      </c>
-      <c r="F57" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F57" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G57" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>74</v>
       </c>
@@ -2177,14 +2416,14 @@
       <c r="D58" t="s">
         <v>2</v>
       </c>
-      <c r="E58" t="s">
-        <v>109</v>
-      </c>
-      <c r="F58" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F58" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G58" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>74</v>
       </c>
@@ -2197,14 +2436,14 @@
       <c r="D59" t="s">
         <v>15</v>
       </c>
-      <c r="E59" t="s">
-        <v>109</v>
-      </c>
-      <c r="F59" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F59" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G59" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>74</v>
       </c>
@@ -2217,14 +2456,14 @@
       <c r="D60" t="s">
         <v>15</v>
       </c>
-      <c r="E60" t="s">
-        <v>109</v>
-      </c>
-      <c r="F60" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F60" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G60" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>74</v>
       </c>
@@ -2237,14 +2476,14 @@
       <c r="D61" t="s">
         <v>2</v>
       </c>
-      <c r="E61" t="s">
-        <v>109</v>
-      </c>
-      <c r="F61" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F61" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G61" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>74</v>
       </c>
@@ -2257,14 +2496,14 @@
       <c r="D62" t="s">
         <v>2</v>
       </c>
-      <c r="E62" t="s">
-        <v>109</v>
-      </c>
-      <c r="F62" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F62" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G62" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>74</v>
       </c>
@@ -2277,14 +2516,14 @@
       <c r="D63" t="s">
         <v>15</v>
       </c>
-      <c r="E63" t="s">
-        <v>109</v>
-      </c>
-      <c r="F63" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F63" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G63" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>74</v>
       </c>
@@ -2297,14 +2536,14 @@
       <c r="D64" t="s">
         <v>2</v>
       </c>
-      <c r="E64" t="s">
-        <v>109</v>
-      </c>
-      <c r="F64" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F64" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G64" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>74</v>
       </c>
@@ -2317,10 +2556,10 @@
       <c r="D65" t="s">
         <v>15</v>
       </c>
-      <c r="E65" t="s">
-        <v>109</v>
-      </c>
-      <c r="F65" t="s">
+      <c r="F65" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G65" s="6" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[MDTUDDM-28611] - Added xms xmx values for java services where missed
Change-Id: If0c97cae3bb293c78882fd5471f1d41a31569bc8
</commit_message>
<xml_diff>
--- a/docs/ua/modules/arch/attachments/architecture/platform-system-requirements/registry-resources.xlsx
+++ b/docs/ua/modules/arch/attachments/architecture/platform-system-requirements/registry-resources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Maksym_Kharchenko/Work/Development/mdtu-ddm/mdtu-ddm-gerrit-workspace/mdtu-ddm/general/ddm-architecture/docs/ua/modules/arch/attachments/architecture/platform-system-requirements/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\mdtu-ddm\ddm-architecture\docs\ua\modules\arch\attachments\architecture\platform-system-requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A966E22-16E8-1D45-9C87-2BA7147D04B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58696646-35AE-4678-84B7-6FBAB89169CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="760" windowWidth="29940" windowHeight="21580" xr2:uid="{76BACE1B-BDCC-F34F-9205-7BB42BE8027F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{76BACE1B-BDCC-F34F-9205-7BB42BE8027F}"/>
   </bookViews>
   <sheets>
     <sheet name="Registry Resources" sheetId="2" r:id="rId1"/>
@@ -519,7 +519,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -541,9 +541,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
@@ -576,6 +573,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -585,7 +600,7 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -594,7 +609,7 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -669,6 +684,9 @@
       </customFilters>
     </filterColumn>
   </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:U58">
+    <sortCondition ref="C1:C65"/>
+  </sortState>
   <tableColumns count="21">
     <tableColumn id="1" xr3:uid="{7B40E2F0-02D6-904B-8018-66FABFA0DD1D}" name="Zone" dataDxfId="20"/>
     <tableColumn id="2" xr3:uid="{9B6E3613-3147-0A49-A88D-DE5E5756377A}" name="Subsystem" dataDxfId="19"/>
@@ -686,11 +704,11 @@
     <tableColumn id="7" xr3:uid="{7D3E02CE-7CDD-5E44-88DF-1162888AE695}" name="-Xms, Mb (baseline)" dataDxfId="7"/>
     <tableColumn id="8" xr3:uid="{3D28B649-AB9D-9C49-8889-6B0D4888A8D3}" name="-Xmx, Mb (baseline)" dataDxfId="6"/>
     <tableColumn id="13" xr3:uid="{729BA2AA-0236-6D4E-88FA-AF5279155852}" name="-Xmn, Mb (baseline)" dataDxfId="5"/>
-    <tableColumn id="21" xr3:uid="{0E115C8F-10F3-1849-9086-23ECFF100762}" name="-Xms, Mb (target)" dataDxfId="0"/>
-    <tableColumn id="20" xr3:uid="{59ED4565-1835-554A-B6BE-EFEE9FF75498}" name="-Xmx, Mb (target)" dataDxfId="1"/>
+    <tableColumn id="21" xr3:uid="{0E115C8F-10F3-1849-9086-23ECFF100762}" name="-Xms, Mb (target)" dataDxfId="4"/>
+    <tableColumn id="20" xr3:uid="{59ED4565-1835-554A-B6BE-EFEE9FF75498}" name="-Xmx, Mb (target)" dataDxfId="3"/>
     <tableColumn id="19" xr3:uid="{5B7661BC-38C4-754F-9E3A-2E5DFADC19B1}" name="-Xmn, Mb (target)" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{84FF7781-94A1-1246-98C1-52FEAF154639}" name="Java Opts (baseline)" dataDxfId="4"/>
-    <tableColumn id="18" xr3:uid="{8EF485D1-BA5B-0B42-B711-53E12FB7661E}" name="Java Opts (target)" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{84FF7781-94A1-1246-98C1-52FEAF154639}" name="Java Opts (baseline)" dataDxfId="1"/>
+    <tableColumn id="18" xr3:uid="{8EF485D1-BA5B-0B42-B711-53E12FB7661E}" name="Java Opts (target)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -995,35 +1013,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C809D083-7CF6-1445-A306-E810BD791428}">
   <dimension ref="A1:U65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="108" workbookViewId="0">
+      <selection activeCell="R31" sqref="R31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.83203125" customWidth="1"/>
-    <col min="2" max="2" width="65.83203125" customWidth="1"/>
+    <col min="1" max="1" width="28.796875" customWidth="1"/>
+    <col min="2" max="2" width="65.796875" customWidth="1"/>
     <col min="3" max="3" width="35.5" customWidth="1"/>
-    <col min="4" max="5" width="19.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" style="2" customWidth="1"/>
+    <col min="4" max="5" width="19.69921875" customWidth="1"/>
+    <col min="6" max="6" width="14.296875" style="2" customWidth="1"/>
     <col min="7" max="7" width="15.5" style="2" customWidth="1"/>
     <col min="8" max="8" width="15.5" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="18.83203125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="14.296875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="18.796875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="14.69921875" style="2" customWidth="1"/>
     <col min="12" max="12" width="21" style="2" customWidth="1"/>
-    <col min="13" max="13" width="21.33203125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="21.296875" style="2" customWidth="1"/>
     <col min="14" max="14" width="21.5" customWidth="1"/>
-    <col min="15" max="15" width="19.83203125" customWidth="1"/>
+    <col min="15" max="15" width="19.796875" customWidth="1"/>
     <col min="16" max="16" width="20.5" customWidth="1"/>
     <col min="17" max="17" width="19.5" customWidth="1"/>
-    <col min="18" max="18" width="18.1640625" customWidth="1"/>
+    <col min="18" max="18" width="18.19921875" customWidth="1"/>
     <col min="19" max="19" width="18.5" customWidth="1"/>
-    <col min="20" max="20" width="65.6640625" customWidth="1"/>
-    <col min="21" max="21" width="66.6640625" style="3" customWidth="1"/>
+    <col min="20" max="20" width="65.69921875" customWidth="1"/>
+    <col min="21" max="21" width="66.69921875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>96</v>
       </c>
@@ -1088,7 +1106,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" ht="16.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>73</v>
       </c>
@@ -1117,7 +1135,7 @@
         <v>110</v>
       </c>
       <c r="L2" s="6"/>
-      <c r="M2" s="13" t="s">
+      <c r="M2" s="12" t="s">
         <v>113</v>
       </c>
       <c r="N2" s="4"/>
@@ -1129,7 +1147,7 @@
       <c r="T2" s="4"/>
       <c r="U2" s="6"/>
     </row>
-    <row r="3" spans="1:21" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="16.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>73</v>
       </c>
@@ -1158,7 +1176,7 @@
         <v>110</v>
       </c>
       <c r="L3" s="6"/>
-      <c r="M3" s="13" t="s">
+      <c r="M3" s="12" t="s">
         <v>113</v>
       </c>
       <c r="N3" s="4"/>
@@ -1170,7 +1188,7 @@
       <c r="T3" s="4"/>
       <c r="U3" s="6"/>
     </row>
-    <row r="4" spans="1:21" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" ht="16.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>73</v>
       </c>
@@ -1199,7 +1217,7 @@
         <v>110</v>
       </c>
       <c r="L4" s="6"/>
-      <c r="M4" s="13" t="s">
+      <c r="M4" s="12" t="s">
         <v>113</v>
       </c>
       <c r="N4" s="4"/>
@@ -1211,7 +1229,7 @@
       <c r="T4" s="4"/>
       <c r="U4" s="6"/>
     </row>
-    <row r="5" spans="1:21" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" ht="16.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>73</v>
       </c>
@@ -1240,7 +1258,7 @@
         <v>110</v>
       </c>
       <c r="L5" s="6"/>
-      <c r="M5" s="13" t="s">
+      <c r="M5" s="12" t="s">
         <v>113</v>
       </c>
       <c r="N5" s="4"/>
@@ -1252,15 +1270,15 @@
       <c r="T5" s="4"/>
       <c r="U5" s="6"/>
     </row>
-    <row r="6" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>15</v>
@@ -1282,17 +1300,17 @@
       <c r="K6" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="L6" s="12" t="s">
+      <c r="L6" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="M6" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="N6" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="O6" s="14" t="s">
-        <v>114</v>
+      <c r="M6" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="N6" s="18">
+        <v>1536</v>
+      </c>
+      <c r="O6" s="18">
+        <v>1536</v>
       </c>
       <c r="P6" s="6" t="s">
         <v>9</v>
@@ -1300,14 +1318,14 @@
       <c r="Q6" s="6"/>
       <c r="R6" s="6"/>
       <c r="S6" s="6"/>
-      <c r="T6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="U6" s="17" t="s">
+      <c r="T6" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="U6" s="16" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" ht="16.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>73</v>
       </c>
@@ -1336,7 +1354,7 @@
         <v>110</v>
       </c>
       <c r="L7" s="6"/>
-      <c r="M7" s="13" t="s">
+      <c r="M7" s="12" t="s">
         <v>113</v>
       </c>
       <c r="N7" s="4"/>
@@ -1348,7 +1366,7 @@
       <c r="T7" s="4"/>
       <c r="U7" s="6"/>
     </row>
-    <row r="8" spans="1:21" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" ht="16.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>73</v>
       </c>
@@ -1377,7 +1395,7 @@
         <v>110</v>
       </c>
       <c r="L8" s="6"/>
-      <c r="M8" s="13" t="s">
+      <c r="M8" s="12" t="s">
         <v>113</v>
       </c>
       <c r="N8" s="4"/>
@@ -1389,7 +1407,7 @@
       <c r="T8" s="4"/>
       <c r="U8" s="6"/>
     </row>
-    <row r="9" spans="1:21" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" ht="16.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>73</v>
       </c>
@@ -1418,7 +1436,7 @@
         <v>110</v>
       </c>
       <c r="L9" s="6"/>
-      <c r="M9" s="13" t="s">
+      <c r="M9" s="12" t="s">
         <v>113</v>
       </c>
       <c r="N9" s="4"/>
@@ -1430,7 +1448,7 @@
       <c r="T9" s="4"/>
       <c r="U9" s="6"/>
     </row>
-    <row r="10" spans="1:21" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" ht="16.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>73</v>
       </c>
@@ -1459,7 +1477,7 @@
         <v>110</v>
       </c>
       <c r="L10" s="6"/>
-      <c r="M10" s="13" t="s">
+      <c r="M10" s="12" t="s">
         <v>113</v>
       </c>
       <c r="N10" s="4"/>
@@ -1471,15 +1489,15 @@
       <c r="T10" s="4"/>
       <c r="U10" s="6"/>
     </row>
-    <row r="11" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>15</v>
@@ -1501,17 +1519,17 @@
       <c r="K11" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="L11" s="12" t="s">
+      <c r="L11" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="M11" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="N11" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="O11" s="14" t="s">
-        <v>114</v>
+      <c r="M11" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="N11" s="18">
+        <v>512</v>
+      </c>
+      <c r="O11" s="18">
+        <v>512</v>
       </c>
       <c r="P11" s="6" t="s">
         <v>9</v>
@@ -1522,19 +1540,19 @@
       <c r="T11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="U11" s="17" t="s">
+      <c r="U11" s="16" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>73</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>15</v>
@@ -1544,7 +1562,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="6" t="s">
@@ -1556,17 +1574,17 @@
       <c r="K12" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="L12" s="12" t="s">
+      <c r="L12" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="M12" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="N12" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="O12" s="14" t="s">
-        <v>114</v>
+      <c r="M12" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="N12" s="18">
+        <v>512</v>
+      </c>
+      <c r="O12" s="18">
+        <v>512</v>
       </c>
       <c r="P12" s="6" t="s">
         <v>9</v>
@@ -1577,11 +1595,11 @@
       <c r="T12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="U12" s="17" t="s">
+      <c r="U12" s="16" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="13" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>73</v>
       </c>
@@ -1610,7 +1628,7 @@
         <v>110</v>
       </c>
       <c r="L13" s="6"/>
-      <c r="M13" s="13" t="s">
+      <c r="M13" s="12" t="s">
         <v>113</v>
       </c>
       <c r="N13" s="4"/>
@@ -1622,7 +1640,7 @@
       <c r="T13" s="4"/>
       <c r="U13" s="6"/>
     </row>
-    <row r="14" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>73</v>
       </c>
@@ -1651,7 +1669,7 @@
         <v>110</v>
       </c>
       <c r="L14" s="6"/>
-      <c r="M14" s="13" t="s">
+      <c r="M14" s="12" t="s">
         <v>113</v>
       </c>
       <c r="N14" s="4"/>
@@ -1663,15 +1681,15 @@
       <c r="T14" s="4"/>
       <c r="U14" s="6"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>73</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>18</v>
+        <v>70</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>20</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>15</v>
@@ -1681,7 +1699,7 @@
         <v>3</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="6" t="s">
@@ -1693,40 +1711,44 @@
       <c r="K15" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="L15" s="12" t="s">
+      <c r="L15" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="M15" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="N15" s="19">
-        <v>512</v>
-      </c>
-      <c r="O15" s="19">
-        <v>512</v>
+      <c r="M15" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="N15" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="O15" s="13" t="s">
+        <v>114</v>
       </c>
       <c r="P15" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="Q15" s="6"/>
-      <c r="R15" s="6"/>
+      <c r="Q15" s="6">
+        <v>600</v>
+      </c>
+      <c r="R15" s="6">
+        <v>600</v>
+      </c>
       <c r="S15" s="6"/>
       <c r="T15" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="U15" s="17" t="s">
+      <c r="U15" s="16" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>15</v>
@@ -1736,7 +1758,7 @@
         <v>3</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="6" t="s">
@@ -1748,32 +1770,36 @@
       <c r="K16" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="L16" s="12" t="s">
+      <c r="L16" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="M16" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="N16" s="18" t="s">
+      <c r="M16" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="N16" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="O16" s="18" t="s">
+      <c r="O16" s="17" t="s">
         <v>114</v>
       </c>
       <c r="P16" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="Q16" s="6"/>
-      <c r="R16" s="6"/>
+      <c r="Q16" s="6">
+        <v>500</v>
+      </c>
+      <c r="R16" s="6">
+        <v>500</v>
+      </c>
       <c r="S16" s="6"/>
       <c r="T16" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="U16" s="17" t="s">
+      <c r="U16" s="16" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="17" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>73</v>
       </c>
@@ -1802,7 +1828,7 @@
         <v>110</v>
       </c>
       <c r="L17" s="6"/>
-      <c r="M17" s="13" t="s">
+      <c r="M17" s="12" t="s">
         <v>113</v>
       </c>
       <c r="N17" s="4"/>
@@ -1814,7 +1840,7 @@
       <c r="T17" s="4"/>
       <c r="U17" s="6"/>
     </row>
-    <row r="18" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>74</v>
       </c>
@@ -1843,7 +1869,7 @@
         <v>110</v>
       </c>
       <c r="L18" s="6"/>
-      <c r="M18" s="13" t="s">
+      <c r="M18" s="12" t="s">
         <v>113</v>
       </c>
       <c r="N18" s="4"/>
@@ -1855,7 +1881,7 @@
       <c r="T18" s="4"/>
       <c r="U18" s="6"/>
     </row>
-    <row r="19" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>74</v>
       </c>
@@ -1884,7 +1910,7 @@
         <v>110</v>
       </c>
       <c r="L19" s="6"/>
-      <c r="M19" s="13" t="s">
+      <c r="M19" s="12" t="s">
         <v>113</v>
       </c>
       <c r="N19" s="4"/>
@@ -1896,7 +1922,7 @@
       <c r="T19" s="4"/>
       <c r="U19" s="6"/>
     </row>
-    <row r="20" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>74</v>
       </c>
@@ -1925,7 +1951,7 @@
         <v>110</v>
       </c>
       <c r="L20" s="6"/>
-      <c r="M20" s="13" t="s">
+      <c r="M20" s="12" t="s">
         <v>113</v>
       </c>
       <c r="N20" s="4"/>
@@ -1937,7 +1963,7 @@
       <c r="T20" s="4"/>
       <c r="U20" s="6"/>
     </row>
-    <row r="21" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>74</v>
       </c>
@@ -1966,7 +1992,7 @@
         <v>110</v>
       </c>
       <c r="L21" s="6"/>
-      <c r="M21" s="13" t="s">
+      <c r="M21" s="12" t="s">
         <v>113</v>
       </c>
       <c r="N21" s="4"/>
@@ -1978,7 +2004,7 @@
       <c r="T21" s="4"/>
       <c r="U21" s="6"/>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>74</v>
       </c>
@@ -1986,7 +2012,7 @@
         <v>77</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>15</v>
@@ -2008,17 +2034,17 @@
       <c r="K22" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="L22" s="12" t="s">
+      <c r="L22" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="M22" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="N22" s="19">
-        <v>1536</v>
-      </c>
-      <c r="O22" s="19">
-        <v>1536</v>
+      <c r="M22" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="N22" s="18">
+        <v>512</v>
+      </c>
+      <c r="O22" s="18">
+        <v>512</v>
       </c>
       <c r="P22" s="6" t="s">
         <v>9</v>
@@ -2026,22 +2052,22 @@
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
       <c r="S22" s="6"/>
-      <c r="T22" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="U22" s="17" t="s">
+      <c r="T22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="U22" s="16" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>15</v>
@@ -2051,7 +2077,7 @@
         <v>3</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="H23" s="4"/>
       <c r="I23" s="6" t="s">
@@ -2063,17 +2089,17 @@
       <c r="K23" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="L23" s="12" t="s">
+      <c r="L23" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="M23" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="N23" s="19">
-        <v>512</v>
-      </c>
-      <c r="O23" s="19">
-        <v>512</v>
+      <c r="M23" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="N23" s="18">
+        <v>768</v>
+      </c>
+      <c r="O23" s="18">
+        <v>768</v>
       </c>
       <c r="P23" s="6" t="s">
         <v>9</v>
@@ -2082,21 +2108,21 @@
       <c r="R23" s="6"/>
       <c r="S23" s="6"/>
       <c r="T23" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="U23" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="U23" s="16" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>28</v>
+        <v>82</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>24</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>15</v>
@@ -2118,32 +2144,32 @@
       <c r="K24" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="L24" s="12" t="s">
+      <c r="L24" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="M24" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="N24" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="O24" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="P24" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q24" s="6"/>
-      <c r="R24" s="6"/>
-      <c r="S24" s="6"/>
-      <c r="T24" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="U24" s="17" t="s">
+      <c r="M24" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="N24" s="23">
+        <v>330</v>
+      </c>
+      <c r="O24" s="23">
+        <v>330</v>
+      </c>
+      <c r="P24" s="13">
+        <v>200</v>
+      </c>
+      <c r="Q24" s="13"/>
+      <c r="R24" s="13"/>
+      <c r="S24" s="13"/>
+      <c r="T24" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="U24" s="16" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="25" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>74</v>
       </c>
@@ -2172,7 +2198,7 @@
         <v>110</v>
       </c>
       <c r="L25" s="6"/>
-      <c r="M25" s="13" t="s">
+      <c r="M25" s="12" t="s">
         <v>113</v>
       </c>
       <c r="N25" s="4"/>
@@ -2184,15 +2210,15 @@
       <c r="T25" s="4"/>
       <c r="U25" s="6"/>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>15</v>
@@ -2214,40 +2240,40 @@
       <c r="K26" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="L26" s="12" t="s">
+      <c r="L26" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="M26" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="N26" s="19">
+      <c r="M26" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="N26" s="18">
         <v>330</v>
       </c>
-      <c r="O26" s="19">
+      <c r="O26" s="18">
         <v>330</v>
       </c>
-      <c r="P26" s="14">
+      <c r="P26" s="13">
         <v>200</v>
       </c>
-      <c r="Q26" s="14"/>
-      <c r="R26" s="14"/>
-      <c r="S26" s="14"/>
+      <c r="Q26" s="13"/>
+      <c r="R26" s="13"/>
+      <c r="S26" s="13"/>
       <c r="T26" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="U26" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="U26" s="16" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>15</v>
@@ -2269,40 +2295,40 @@
       <c r="K27" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="L27" s="12" t="s">
+      <c r="L27" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="M27" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="N27" s="19">
+      <c r="M27" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="N27" s="18">
         <v>330</v>
       </c>
-      <c r="O27" s="19">
+      <c r="O27" s="18">
         <v>330</v>
       </c>
-      <c r="P27" s="14">
+      <c r="P27" s="13">
         <v>200</v>
       </c>
-      <c r="Q27" s="14"/>
-      <c r="R27" s="14"/>
-      <c r="S27" s="14"/>
+      <c r="Q27" s="13"/>
+      <c r="R27" s="13"/>
+      <c r="S27" s="13"/>
       <c r="T27" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="U27" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="U27" s="16" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>15</v>
@@ -2324,32 +2350,32 @@
       <c r="K28" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="L28" s="12" t="s">
+      <c r="L28" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="M28" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="N28" s="19">
-        <v>512</v>
-      </c>
-      <c r="O28" s="19">
-        <v>512</v>
-      </c>
-      <c r="P28" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q28" s="6"/>
-      <c r="R28" s="6"/>
-      <c r="S28" s="6"/>
-      <c r="T28" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="U28" s="17" t="s">
+      <c r="M28" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="N28" s="18">
+        <v>330</v>
+      </c>
+      <c r="O28" s="18">
+        <v>330</v>
+      </c>
+      <c r="P28" s="13">
+        <v>200</v>
+      </c>
+      <c r="Q28" s="13"/>
+      <c r="R28" s="13"/>
+      <c r="S28" s="13"/>
+      <c r="T28" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="U28" s="16" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>74</v>
       </c>
@@ -2357,7 +2383,7 @@
         <v>77</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>15</v>
@@ -2379,47 +2405,51 @@
       <c r="K29" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="L29" s="12" t="s">
+      <c r="L29" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="M29" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="N29" s="19">
+      <c r="M29" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="N29" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="O29" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="P29" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q29" s="6">
         <v>512</v>
       </c>
-      <c r="O29" s="19">
+      <c r="R29" s="6">
         <v>512</v>
       </c>
-      <c r="P29" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q29" s="6"/>
-      <c r="R29" s="6"/>
       <c r="S29" s="6"/>
       <c r="T29" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="U29" s="17" t="s">
+      <c r="U29" s="16" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="6" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="G30" s="6" t="s">
         <v>3</v>
@@ -2434,50 +2464,54 @@
       <c r="K30" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="L30" s="12" t="s">
+      <c r="L30" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="M30" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="N30" s="19">
-        <v>1200</v>
-      </c>
-      <c r="O30" s="19">
-        <v>1200</v>
+      <c r="M30" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="N30" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="O30" s="22" t="s">
+        <v>114</v>
       </c>
       <c r="P30" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="Q30" s="6"/>
-      <c r="R30" s="6"/>
+      <c r="Q30" s="6">
+        <v>700</v>
+      </c>
+      <c r="R30" s="6">
+        <v>700</v>
+      </c>
       <c r="S30" s="6"/>
-      <c r="T30" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="U30" s="17" t="s">
+      <c r="T30" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="U30" s="16" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:21" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>57</v>
+        <v>89</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>5</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="H31" s="4"/>
       <c r="I31" s="6" t="s">
@@ -2489,32 +2523,32 @@
       <c r="K31" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="L31" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="M31" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="N31" s="19">
-        <v>1200</v>
-      </c>
-      <c r="O31" s="19">
-        <v>1200</v>
-      </c>
-      <c r="P31" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q31" s="6"/>
-      <c r="R31" s="6"/>
+      <c r="L31" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="M31" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="N31" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="O31" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="P31" s="6"/>
+      <c r="Q31" s="6">
+        <v>512</v>
+      </c>
+      <c r="R31" s="6">
+        <v>3096</v>
+      </c>
       <c r="S31" s="6"/>
-      <c r="T31" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="U31" s="17" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+      <c r="T31" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="U31" s="16"/>
+    </row>
+    <row r="32" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>74</v>
       </c>
@@ -2543,7 +2577,7 @@
         <v>110</v>
       </c>
       <c r="L32" s="6"/>
-      <c r="M32" s="13" t="s">
+      <c r="M32" s="12" t="s">
         <v>113</v>
       </c>
       <c r="N32" s="4"/>
@@ -2555,7 +2589,7 @@
       <c r="T32" s="4"/>
       <c r="U32" s="6"/>
     </row>
-    <row r="33" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>74</v>
       </c>
@@ -2584,7 +2618,7 @@
         <v>110</v>
       </c>
       <c r="L33" s="6"/>
-      <c r="M33" s="13" t="s">
+      <c r="M33" s="12" t="s">
         <v>113</v>
       </c>
       <c r="N33" s="4"/>
@@ -2596,7 +2630,7 @@
       <c r="T33" s="4"/>
       <c r="U33" s="6"/>
     </row>
-    <row r="34" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>74</v>
       </c>
@@ -2625,7 +2659,7 @@
         <v>110</v>
       </c>
       <c r="L34" s="6"/>
-      <c r="M34" s="13" t="s">
+      <c r="M34" s="12" t="s">
         <v>113</v>
       </c>
       <c r="N34" s="4"/>
@@ -2637,7 +2671,7 @@
       <c r="T34" s="4"/>
       <c r="U34" s="6"/>
     </row>
-    <row r="35" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>74</v>
       </c>
@@ -2666,7 +2700,7 @@
         <v>110</v>
       </c>
       <c r="L35" s="6"/>
-      <c r="M35" s="13" t="s">
+      <c r="M35" s="12" t="s">
         <v>113</v>
       </c>
       <c r="N35" s="4"/>
@@ -2678,7 +2712,7 @@
       <c r="T35" s="4"/>
       <c r="U35" s="6"/>
     </row>
-    <row r="36" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>74</v>
       </c>
@@ -2707,7 +2741,7 @@
         <v>110</v>
       </c>
       <c r="L36" s="6"/>
-      <c r="M36" s="13" t="s">
+      <c r="M36" s="12" t="s">
         <v>113</v>
       </c>
       <c r="N36" s="4"/>
@@ -2719,7 +2753,7 @@
       <c r="T36" s="4"/>
       <c r="U36" s="6"/>
     </row>
-    <row r="37" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>74</v>
       </c>
@@ -2748,7 +2782,7 @@
         <v>110</v>
       </c>
       <c r="L37" s="6"/>
-      <c r="M37" s="13" t="s">
+      <c r="M37" s="12" t="s">
         <v>113</v>
       </c>
       <c r="N37" s="4"/>
@@ -2760,25 +2794,25 @@
       <c r="T37" s="4"/>
       <c r="U37" s="6"/>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="H38" s="4"/>
       <c r="I38" s="6" t="s">
@@ -2790,40 +2824,38 @@
       <c r="K38" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="L38" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="M38" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="N38" s="19">
-        <v>512</v>
-      </c>
-      <c r="O38" s="19">
-        <v>512</v>
-      </c>
-      <c r="P38" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q38" s="6"/>
-      <c r="R38" s="6"/>
+      <c r="L38" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="M38" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="N38" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="O38" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="P38" s="6"/>
+      <c r="Q38" s="6">
+        <v>400</v>
+      </c>
+      <c r="R38" s="6">
+        <v>400</v>
+      </c>
       <c r="S38" s="6"/>
-      <c r="T38" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="U38" s="17" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="T38" s="4"/>
+      <c r="U38" s="16"/>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>15</v>
@@ -2833,7 +2865,7 @@
         <v>3</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="H39" s="4"/>
       <c r="I39" s="6" t="s">
@@ -2845,32 +2877,36 @@
       <c r="K39" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="L39" s="12" t="s">
+      <c r="L39" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="M39" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="N39" s="19">
-        <v>330</v>
-      </c>
-      <c r="O39" s="19">
-        <v>330</v>
-      </c>
-      <c r="P39" s="14">
-        <v>200</v>
-      </c>
-      <c r="Q39" s="14"/>
-      <c r="R39" s="14"/>
-      <c r="S39" s="14"/>
-      <c r="T39" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="U39" s="17" t="s">
+      <c r="M39" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="N39" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="O39" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="P39" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q39" s="6">
+        <v>300</v>
+      </c>
+      <c r="R39" s="6">
+        <v>300</v>
+      </c>
+      <c r="S39" s="6"/>
+      <c r="T39" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="U39" s="16" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>74</v>
       </c>
@@ -2878,14 +2914,14 @@
         <v>80</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="6" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G40" s="6" t="s">
         <v>3</v>
@@ -2900,47 +2936,47 @@
       <c r="K40" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="L40" s="12" t="s">
+      <c r="L40" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="M40" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="N40" s="19">
-        <v>1200</v>
-      </c>
-      <c r="O40" s="19">
-        <v>1200</v>
-      </c>
-      <c r="P40" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q40" s="6"/>
-      <c r="R40" s="6"/>
-      <c r="S40" s="6"/>
-      <c r="T40" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="U40" s="17" t="s">
+      <c r="M40" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="N40" s="18">
+        <v>330</v>
+      </c>
+      <c r="O40" s="18">
+        <v>330</v>
+      </c>
+      <c r="P40" s="13">
+        <v>200</v>
+      </c>
+      <c r="Q40" s="13"/>
+      <c r="R40" s="13"/>
+      <c r="S40" s="13"/>
+      <c r="T40" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="U40" s="16" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="6" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G41" s="6" t="s">
         <v>3</v>
@@ -2955,47 +2991,47 @@
       <c r="K41" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="L41" s="12" t="s">
+      <c r="L41" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="M41" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="N41" s="19">
-        <v>1200</v>
-      </c>
-      <c r="O41" s="19">
-        <v>1200</v>
-      </c>
-      <c r="P41" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q41" s="6"/>
-      <c r="R41" s="6"/>
-      <c r="S41" s="6"/>
-      <c r="T41" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="U41" s="17" t="s">
+      <c r="M41" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="N41" s="18">
+        <v>330</v>
+      </c>
+      <c r="O41" s="18">
+        <v>330</v>
+      </c>
+      <c r="P41" s="13">
+        <v>200</v>
+      </c>
+      <c r="Q41" s="13"/>
+      <c r="R41" s="13"/>
+      <c r="S41" s="13"/>
+      <c r="T41" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="U41" s="16" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="6" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G42" s="6" t="s">
         <v>3</v>
@@ -3010,40 +3046,40 @@
       <c r="K42" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="L42" s="12" t="s">
+      <c r="L42" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="M42" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="N42" s="19">
-        <v>128</v>
-      </c>
-      <c r="O42" s="19">
-        <v>128</v>
-      </c>
-      <c r="P42" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q42" s="6"/>
-      <c r="R42" s="6"/>
-      <c r="S42" s="6"/>
-      <c r="T42" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="U42" s="17" t="s">
+      <c r="M42" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="N42" s="18">
+        <v>330</v>
+      </c>
+      <c r="O42" s="18">
+        <v>330</v>
+      </c>
+      <c r="P42" s="13">
+        <v>200</v>
+      </c>
+      <c r="Q42" s="13"/>
+      <c r="R42" s="13"/>
+      <c r="S42" s="13"/>
+      <c r="T42" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="U42" s="16" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>15</v>
@@ -3053,7 +3089,7 @@
         <v>3</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="H43" s="4"/>
       <c r="I43" s="6" t="s">
@@ -3065,17 +3101,17 @@
       <c r="K43" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="L43" s="12" t="s">
+      <c r="L43" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="M43" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="N43" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="O43" s="18" t="s">
-        <v>114</v>
+      <c r="M43" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="N43" s="23">
+        <v>1200</v>
+      </c>
+      <c r="O43" s="23">
+        <v>1200</v>
       </c>
       <c r="P43" s="6" t="s">
         <v>9</v>
@@ -3083,22 +3119,22 @@
       <c r="Q43" s="6"/>
       <c r="R43" s="6"/>
       <c r="S43" s="6"/>
-      <c r="T43" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="U43" s="17" t="s">
+      <c r="T43" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="U43" s="16" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>24</v>
+        <v>70</v>
+      </c>
+      <c r="C44" s="21" t="s">
+        <v>56</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>15</v>
@@ -3120,40 +3156,44 @@
       <c r="K44" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="L44" s="12" t="s">
+      <c r="L44" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="M44" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="N44" s="19">
-        <v>330</v>
-      </c>
-      <c r="O44" s="19">
-        <v>330</v>
-      </c>
-      <c r="P44" s="14">
-        <v>200</v>
-      </c>
-      <c r="Q44" s="14"/>
-      <c r="R44" s="14"/>
-      <c r="S44" s="14"/>
-      <c r="T44" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="U44" s="17" t="s">
+      <c r="M44" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="N44" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="O44" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="P44" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q44" s="6">
+        <v>900</v>
+      </c>
+      <c r="R44" s="6">
+        <v>900</v>
+      </c>
+      <c r="S44" s="6"/>
+      <c r="T44" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="U44" s="16" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>15</v>
@@ -3175,47 +3215,47 @@
       <c r="K45" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="L45" s="12" t="s">
+      <c r="L45" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="M45" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="N45" s="19">
-        <v>330</v>
-      </c>
-      <c r="O45" s="19">
-        <v>330</v>
-      </c>
-      <c r="P45" s="14">
-        <v>200</v>
-      </c>
-      <c r="Q45" s="14"/>
-      <c r="R45" s="14"/>
-      <c r="S45" s="14"/>
-      <c r="T45" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="U45" s="17" t="s">
+      <c r="M45" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="N45" s="18">
+        <v>1200</v>
+      </c>
+      <c r="O45" s="18">
+        <v>1200</v>
+      </c>
+      <c r="P45" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q45" s="6"/>
+      <c r="R45" s="6"/>
+      <c r="S45" s="6"/>
+      <c r="T45" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="U45" s="16" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="6" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="G46" s="6" t="s">
         <v>3</v>
@@ -3230,47 +3270,47 @@
       <c r="K46" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="L46" s="12" t="s">
+      <c r="L46" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="M46" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="N46" s="19">
-        <v>330</v>
-      </c>
-      <c r="O46" s="19">
-        <v>330</v>
-      </c>
-      <c r="P46" s="14">
-        <v>200</v>
-      </c>
-      <c r="Q46" s="14"/>
-      <c r="R46" s="14"/>
-      <c r="S46" s="14"/>
-      <c r="T46" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="U46" s="17" t="s">
+      <c r="M46" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="N46" s="18">
+        <v>1200</v>
+      </c>
+      <c r="O46" s="18">
+        <v>1200</v>
+      </c>
+      <c r="P46" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q46" s="6"/>
+      <c r="R46" s="6"/>
+      <c r="S46" s="6"/>
+      <c r="T46" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="U46" s="16" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E47" s="4"/>
       <c r="F47" s="6" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="G47" s="6" t="s">
         <v>3</v>
@@ -3285,47 +3325,47 @@
       <c r="K47" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="L47" s="12" t="s">
+      <c r="L47" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="M47" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="N47" s="19">
-        <v>330</v>
-      </c>
-      <c r="O47" s="19">
-        <v>330</v>
-      </c>
-      <c r="P47" s="14">
-        <v>200</v>
-      </c>
-      <c r="Q47" s="14"/>
-      <c r="R47" s="14"/>
-      <c r="S47" s="14"/>
-      <c r="T47" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="U47" s="17" t="s">
+      <c r="M47" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="N47" s="18">
+        <v>1200</v>
+      </c>
+      <c r="O47" s="18">
+        <v>1200</v>
+      </c>
+      <c r="P47" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q47" s="6"/>
+      <c r="R47" s="6"/>
+      <c r="S47" s="6"/>
+      <c r="T47" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="U47" s="16" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>21</v>
+        <v>80</v>
+      </c>
+      <c r="C48" s="19" t="s">
+        <v>60</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E48" s="4"/>
       <c r="F48" s="6" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="G48" s="6" t="s">
         <v>3</v>
@@ -3340,17 +3380,17 @@
       <c r="K48" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="L48" s="12" t="s">
+      <c r="L48" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="M48" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="N48" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="O48" s="18" t="s">
-        <v>114</v>
+      <c r="M48" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="N48" s="23">
+        <v>128</v>
+      </c>
+      <c r="O48" s="23">
+        <v>128</v>
       </c>
       <c r="P48" s="6" t="s">
         <v>9</v>
@@ -3358,29 +3398,29 @@
       <c r="Q48" s="6"/>
       <c r="R48" s="6"/>
       <c r="S48" s="6"/>
-      <c r="T48" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="U48" s="17" t="s">
+      <c r="T48" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="U48" s="16" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>30</v>
+        <v>70</v>
+      </c>
+      <c r="C49" s="19" t="s">
+        <v>62</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="6" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G49" s="6" t="s">
         <v>3</v>
@@ -3395,32 +3435,36 @@
       <c r="K49" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="L49" s="12" t="s">
+      <c r="L49" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="M49" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="N49" s="18" t="s">
+      <c r="M49" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="N49" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="O49" s="18" t="s">
+      <c r="O49" s="24" t="s">
         <v>114</v>
       </c>
       <c r="P49" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="Q49" s="6"/>
-      <c r="R49" s="6"/>
+      <c r="Q49" s="6">
+        <v>400</v>
+      </c>
+      <c r="R49" s="6">
+        <v>400</v>
+      </c>
       <c r="S49" s="6"/>
       <c r="T49" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="U49" s="17" t="s">
+      <c r="U49" s="16" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="50" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>74</v>
       </c>
@@ -3449,7 +3493,7 @@
         <v>110</v>
       </c>
       <c r="L50" s="6"/>
-      <c r="M50" s="13" t="s">
+      <c r="M50" s="12" t="s">
         <v>113</v>
       </c>
       <c r="N50" s="4"/>
@@ -3461,7 +3505,7 @@
       <c r="T50" s="4"/>
       <c r="U50" s="6"/>
     </row>
-    <row r="51" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
         <v>74</v>
       </c>
@@ -3490,7 +3534,7 @@
         <v>110</v>
       </c>
       <c r="L51" s="6"/>
-      <c r="M51" s="13" t="s">
+      <c r="M51" s="12" t="s">
         <v>113</v>
       </c>
       <c r="N51" s="4"/>
@@ -3502,15 +3546,15 @@
       <c r="T51" s="4"/>
       <c r="U51" s="6"/>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>66</v>
+        <v>77</v>
+      </c>
+      <c r="C52" s="19" t="s">
+        <v>64</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>15</v>
@@ -3532,40 +3576,40 @@
       <c r="K52" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="L52" s="12" t="s">
+      <c r="L52" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="M52" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="N52" s="19">
-        <v>330</v>
-      </c>
-      <c r="O52" s="19">
-        <v>330</v>
-      </c>
-      <c r="P52" s="14">
-        <v>200</v>
-      </c>
-      <c r="Q52" s="14"/>
-      <c r="R52" s="14"/>
-      <c r="S52" s="14"/>
-      <c r="T52" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="U52" s="17" t="s">
+      <c r="M52" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="N52" s="18">
+        <v>512</v>
+      </c>
+      <c r="O52" s="18">
+        <v>512</v>
+      </c>
+      <c r="P52" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q52" s="6"/>
+      <c r="R52" s="6"/>
+      <c r="S52" s="6"/>
+      <c r="T52" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="U52" s="16" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>15</v>
@@ -3575,7 +3619,7 @@
         <v>3</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="H53" s="4"/>
       <c r="I53" s="6" t="s">
@@ -3587,32 +3631,32 @@
       <c r="K53" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="L53" s="12" t="s">
+      <c r="L53" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="M53" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="N53" s="19">
-        <v>768</v>
-      </c>
-      <c r="O53" s="19">
-        <v>768</v>
-      </c>
-      <c r="P53" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q53" s="6"/>
-      <c r="R53" s="6"/>
-      <c r="S53" s="6"/>
-      <c r="T53" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="U53" s="17" t="s">
+      <c r="M53" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="N53" s="18">
+        <v>330</v>
+      </c>
+      <c r="O53" s="18">
+        <v>330</v>
+      </c>
+      <c r="P53" s="13">
+        <v>200</v>
+      </c>
+      <c r="Q53" s="13"/>
+      <c r="R53" s="13"/>
+      <c r="S53" s="13"/>
+      <c r="T53" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="U53" s="16" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="54" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
         <v>74</v>
       </c>
@@ -3641,7 +3685,7 @@
         <v>110</v>
       </c>
       <c r="L54" s="6"/>
-      <c r="M54" s="13" t="s">
+      <c r="M54" s="12" t="s">
         <v>113</v>
       </c>
       <c r="N54" s="4"/>
@@ -3653,7 +3697,7 @@
       <c r="T54" s="4"/>
       <c r="U54" s="6"/>
     </row>
-    <row r="55" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>74</v>
       </c>
@@ -3682,7 +3726,7 @@
         <v>110</v>
       </c>
       <c r="L55" s="6"/>
-      <c r="M55" s="13" t="s">
+      <c r="M55" s="12" t="s">
         <v>113</v>
       </c>
       <c r="N55" s="4"/>
@@ -3694,7 +3738,7 @@
       <c r="T55" s="4"/>
       <c r="U55" s="6"/>
     </row>
-    <row r="56" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
         <v>74</v>
       </c>
@@ -3723,7 +3767,7 @@
         <v>110</v>
       </c>
       <c r="L56" s="6"/>
-      <c r="M56" s="13" t="s">
+      <c r="M56" s="12" t="s">
         <v>113</v>
       </c>
       <c r="N56" s="4"/>
@@ -3735,25 +3779,25 @@
       <c r="T56" s="4"/>
       <c r="U56" s="6"/>
     </row>
-    <row r="57" spans="1:21" ht="68" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>5</v>
+        <v>65</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E57" s="4"/>
       <c r="F57" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="H57" s="4"/>
       <c r="I57" s="6" t="s">
@@ -3765,39 +3809,43 @@
       <c r="K57" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="L57" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="M57" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="N57" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="O57" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="P57" s="6"/>
+      <c r="L57" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="M57" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="N57" s="18">
+        <v>512</v>
+      </c>
+      <c r="O57" s="18">
+        <v>512</v>
+      </c>
+      <c r="P57" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="Q57" s="6"/>
       <c r="R57" s="6"/>
       <c r="S57" s="6"/>
-      <c r="T57" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="U57" s="17"/>
-    </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="T57" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="U57" s="16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>6</v>
+        <v>67</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E58" s="4"/>
       <c r="F58" s="6" t="s">
@@ -3816,26 +3864,36 @@
       <c r="K58" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="L58" s="12" t="s">
+      <c r="L58" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="M58" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="N58" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="M58" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="N58" s="14" t="s">
+      <c r="O58" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="O58" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="P58" s="6"/>
-      <c r="Q58" s="6"/>
-      <c r="R58" s="6"/>
+      <c r="P58" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q58" s="6">
+        <v>300</v>
+      </c>
+      <c r="R58" s="6">
+        <v>300</v>
+      </c>
       <c r="S58" s="6"/>
-      <c r="T58" s="4"/>
-      <c r="U58" s="17"/>
-    </row>
-    <row r="59" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+      <c r="T58" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="U58" s="16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
         <v>74</v>
       </c>
@@ -3864,7 +3922,7 @@
         <v>110</v>
       </c>
       <c r="L59" s="6"/>
-      <c r="M59" s="13" t="s">
+      <c r="M59" s="12" t="s">
         <v>113</v>
       </c>
       <c r="N59" s="4"/>
@@ -3876,7 +3934,7 @@
       <c r="T59" s="4"/>
       <c r="U59" s="6"/>
     </row>
-    <row r="60" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
         <v>74</v>
       </c>
@@ -3905,7 +3963,7 @@
         <v>110</v>
       </c>
       <c r="L60" s="6"/>
-      <c r="M60" s="13" t="s">
+      <c r="M60" s="12" t="s">
         <v>113</v>
       </c>
       <c r="N60" s="4"/>
@@ -3917,14 +3975,14 @@
       <c r="T60" s="4"/>
       <c r="U60" s="6"/>
     </row>
-    <row r="61" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C61" s="11" t="s">
+      <c r="C61" s="10" t="s">
         <v>1</v>
       </c>
       <c r="D61" s="4" t="s">
@@ -3946,7 +4004,7 @@
         <v>110</v>
       </c>
       <c r="L61" s="6"/>
-      <c r="M61" s="13" t="s">
+      <c r="M61" s="12" t="s">
         <v>113</v>
       </c>
       <c r="N61" s="4"/>
@@ -3958,7 +4016,7 @@
       <c r="T61" s="4"/>
       <c r="U61" s="6"/>
     </row>
-    <row r="62" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
         <v>74</v>
       </c>
@@ -3987,7 +4045,7 @@
         <v>110</v>
       </c>
       <c r="L62" s="6"/>
-      <c r="M62" s="13" t="s">
+      <c r="M62" s="12" t="s">
         <v>113</v>
       </c>
       <c r="N62" s="4"/>
@@ -3999,7 +4057,7 @@
       <c r="T62" s="4"/>
       <c r="U62" s="6"/>
     </row>
-    <row r="63" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
         <v>74</v>
       </c>
@@ -4028,7 +4086,7 @@
         <v>110</v>
       </c>
       <c r="L63" s="6"/>
-      <c r="M63" s="13" t="s">
+      <c r="M63" s="12" t="s">
         <v>113</v>
       </c>
       <c r="N63" s="4"/>
@@ -4040,7 +4098,7 @@
       <c r="T63" s="4"/>
       <c r="U63" s="6"/>
     </row>
-    <row r="64" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
         <v>74</v>
       </c>
@@ -4069,7 +4127,7 @@
         <v>110</v>
       </c>
       <c r="L64" s="6"/>
-      <c r="M64" s="13" t="s">
+      <c r="M64" s="12" t="s">
         <v>113</v>
       </c>
       <c r="N64" s="4"/>
@@ -4081,7 +4139,7 @@
       <c r="T64" s="4"/>
       <c r="U64" s="6"/>
     </row>
-    <row r="65" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
         <v>74</v>
       </c>
@@ -4110,7 +4168,7 @@
         <v>110</v>
       </c>
       <c r="L65" s="6"/>
-      <c r="M65" s="13" t="s">
+      <c r="M65" s="12" t="s">
         <v>113</v>
       </c>
       <c r="N65" s="4"/>

</xml_diff>